<commit_message>
added tables from 07.11.23
</commit_message>
<xml_diff>
--- a/Year 1 - 2023-2024/Modul 1/Excel/07.11.2023/Сценарии.xlsx
+++ b/Year 1 - 2023-2024/Modul 1/Excel/07.11.2023/Сценарии.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\GitHub\IT\Year 1 - 2023-2024\Modul 1\Excel\07.11.2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9CE9F8-656F-44AD-A9B2-A653081F651D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB36690-BE95-4120-B415-3BFC6D002711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10245" windowHeight="11520" activeTab="5" xr2:uid="{F2292B4E-A2C3-4E12-ADB4-217B2CA67F09}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11610" windowHeight="11520" activeTab="5" xr2:uid="{F2292B4E-A2C3-4E12-ADB4-217B2CA67F09}"/>
   </bookViews>
   <sheets>
     <sheet name="зад. 3" sheetId="1" r:id="rId1"/>
     <sheet name="зад. 4" sheetId="2" r:id="rId2"/>
     <sheet name="зад. 5" sheetId="3" r:id="rId3"/>
     <sheet name="Scenario Summary" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="6" r:id="rId6"/>
+    <sheet name="зад. 3 (2)" sheetId="5" r:id="rId5"/>
+    <sheet name="зад. 4 (2)" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="98">
   <si>
     <t>Определяне на цената</t>
   </si>
@@ -275,6 +275,66 @@
   </si>
   <si>
     <t>Данни за производство и продажба на продукт А</t>
+  </si>
+  <si>
+    <t>Приходи от продажбата на продукт А</t>
+  </si>
+  <si>
+    <t>Променливи разходи</t>
+  </si>
+  <si>
+    <t>Отчет</t>
+  </si>
+  <si>
+    <t>Брой произведени продукти</t>
+  </si>
+  <si>
+    <t>Цена на единица продук без ДДС</t>
+  </si>
+  <si>
+    <t>Цена с ДДС</t>
+  </si>
+  <si>
+    <t>Себестойност на продукцията</t>
+  </si>
+  <si>
+    <t>ДДС</t>
+  </si>
+  <si>
+    <t>Общо приход</t>
+  </si>
+  <si>
+    <t>Разходи за вложени материали в производството на един продукт</t>
+  </si>
+  <si>
+    <t>Разхдоди за производство на един продукт</t>
+  </si>
+  <si>
+    <t>Общо променливи разходи</t>
+  </si>
+  <si>
+    <t>Разходи за работна заплата на административен персонал</t>
+  </si>
+  <si>
+    <t>Разходи за доставка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Разходи за съхранение </t>
+  </si>
+  <si>
+    <t>Разходи за обновяване на оборудване</t>
+  </si>
+  <si>
+    <t>Общо фиксирани разходи</t>
+  </si>
+  <si>
+    <t>Общо приходи</t>
+  </si>
+  <si>
+    <t>Общо разходи</t>
+  </si>
+  <si>
+    <t>Печалба</t>
   </si>
 </sst>
 </file>
@@ -658,13 +718,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -705,22 +766,17 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -735,12 +791,12 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -752,15 +808,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Accent3" xfId="3" builtinId="37"/>
     <cellStyle name="Accent4" xfId="2" builtinId="41"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="4" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -773,10 +834,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1089,10 +1146,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
+      <c r="B1" s="44"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1431,13 +1488,13 @@
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="31">
+      <c r="B7" s="30">
         <v>500</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="30">
         <v>400</v>
       </c>
-      <c r="D7" s="31">
+      <c r="D7" s="30">
         <v>300</v>
       </c>
     </row>
@@ -1445,13 +1502,13 @@
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B8" s="1">
         <v>5000</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="1">
         <v>4000</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="1">
         <v>2000</v>
       </c>
     </row>
@@ -1459,13 +1516,13 @@
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="32">
+      <c r="B9" s="1">
         <v>2000</v>
       </c>
-      <c r="C9" s="32">
+      <c r="C9" s="1">
         <v>3000</v>
       </c>
-      <c r="D9" s="32">
+      <c r="D9" s="1">
         <v>4000</v>
       </c>
     </row>
@@ -1581,458 +1638,457 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
     </row>
     <row r="3" spans="2:7" ht="15.75" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="43" t="s">
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="43" t="s">
+      <c r="G3" s="40" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="22.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="46" t="s">
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="E4" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="46" t="s">
+      <c r="F4" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="G4" s="46" t="s">
+      <c r="G4" s="43" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
     </row>
     <row r="6" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="39"/>
-      <c r="C6" s="39" t="s">
+      <c r="B6" s="36"/>
+      <c r="C6" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="34">
+      <c r="D6" s="31">
         <v>40</v>
       </c>
-      <c r="E6" s="44">
+      <c r="E6" s="41">
         <v>42</v>
       </c>
-      <c r="F6" s="44">
+      <c r="F6" s="41">
         <v>40</v>
       </c>
-      <c r="G6" s="44">
+      <c r="G6" s="41">
         <v>38</v>
       </c>
     </row>
     <row r="7" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="39"/>
-      <c r="C7" s="39" t="s">
+      <c r="B7" s="36"/>
+      <c r="C7" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="31">
         <v>60</v>
       </c>
-      <c r="E7" s="44">
+      <c r="E7" s="41">
         <v>62</v>
       </c>
-      <c r="F7" s="44">
+      <c r="F7" s="41">
         <v>60</v>
       </c>
-      <c r="G7" s="44">
+      <c r="G7" s="41">
         <v>58</v>
       </c>
     </row>
     <row r="8" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="39"/>
-      <c r="C8" s="39" t="s">
+      <c r="B8" s="36"/>
+      <c r="C8" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="34">
+      <c r="D8" s="31">
         <v>80</v>
       </c>
-      <c r="E8" s="44">
+      <c r="E8" s="41">
         <v>83</v>
       </c>
-      <c r="F8" s="44">
+      <c r="F8" s="41">
         <v>80</v>
       </c>
-      <c r="G8" s="44">
+      <c r="G8" s="41">
         <v>78</v>
       </c>
     </row>
     <row r="9" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="39"/>
-      <c r="C9" s="39" t="s">
+      <c r="B9" s="36"/>
+      <c r="C9" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="31">
         <v>60</v>
       </c>
-      <c r="E9" s="44">
+      <c r="E9" s="41">
         <v>63</v>
       </c>
-      <c r="F9" s="44">
+      <c r="F9" s="41">
         <v>60</v>
       </c>
-      <c r="G9" s="44">
+      <c r="G9" s="41">
         <v>58</v>
       </c>
     </row>
     <row r="10" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="39"/>
-      <c r="C10" s="39" t="s">
+      <c r="B10" s="36"/>
+      <c r="C10" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="34">
+      <c r="D10" s="31">
         <v>80</v>
       </c>
-      <c r="E10" s="44">
+      <c r="E10" s="41">
         <v>83</v>
       </c>
-      <c r="F10" s="44">
+      <c r="F10" s="41">
         <v>80</v>
       </c>
-      <c r="G10" s="44">
+      <c r="G10" s="41">
         <v>78</v>
       </c>
     </row>
     <row r="11" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="39"/>
-      <c r="C11" s="39" t="s">
+      <c r="B11" s="36"/>
+      <c r="C11" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="34">
+      <c r="D11" s="31">
         <v>100</v>
       </c>
-      <c r="E11" s="44">
+      <c r="E11" s="41">
         <v>102</v>
       </c>
-      <c r="F11" s="44">
+      <c r="F11" s="41">
         <v>100</v>
       </c>
-      <c r="G11" s="44">
+      <c r="G11" s="41">
         <v>98</v>
       </c>
     </row>
     <row r="12" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="39"/>
-      <c r="C12" s="39" t="s">
+      <c r="B12" s="36"/>
+      <c r="C12" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="34">
+      <c r="D12" s="31">
         <v>80</v>
       </c>
-      <c r="E12" s="44">
+      <c r="E12" s="41">
         <v>82</v>
       </c>
-      <c r="F12" s="44">
+      <c r="F12" s="41">
         <v>80</v>
       </c>
-      <c r="G12" s="44">
+      <c r="G12" s="41">
         <v>78</v>
       </c>
     </row>
     <row r="13" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="39"/>
-      <c r="C13" s="39" t="s">
+      <c r="B13" s="36"/>
+      <c r="C13" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="34">
+      <c r="D13" s="31">
         <v>100</v>
       </c>
-      <c r="E13" s="44">
+      <c r="E13" s="41">
         <v>102</v>
       </c>
-      <c r="F13" s="44">
+      <c r="F13" s="41">
         <v>100</v>
       </c>
-      <c r="G13" s="44">
+      <c r="G13" s="41">
         <v>98</v>
       </c>
     </row>
     <row r="14" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="39"/>
-      <c r="C14" s="39" t="s">
+      <c r="B14" s="36"/>
+      <c r="C14" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="34">
+      <c r="D14" s="31">
         <v>120</v>
       </c>
-      <c r="E14" s="44">
+      <c r="E14" s="41">
         <v>122</v>
       </c>
-      <c r="F14" s="44">
+      <c r="F14" s="41">
         <v>120</v>
       </c>
-      <c r="G14" s="44">
+      <c r="G14" s="41">
         <v>118</v>
       </c>
     </row>
     <row r="15" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="39"/>
-      <c r="C15" s="39" t="s">
+      <c r="B15" s="36"/>
+      <c r="C15" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="33">
+      <c r="D15">
         <v>500</v>
       </c>
-      <c r="E15" s="45">
+      <c r="E15" s="42">
         <v>510</v>
       </c>
-      <c r="F15" s="45">
+      <c r="F15" s="42">
         <v>500</v>
       </c>
-      <c r="G15" s="45">
+      <c r="G15" s="42">
         <v>490</v>
       </c>
     </row>
     <row r="16" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="39"/>
-      <c r="C16" s="39" t="s">
+      <c r="B16" s="36"/>
+      <c r="C16" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="33">
+      <c r="D16">
         <v>400</v>
       </c>
-      <c r="E16" s="45">
+      <c r="E16" s="42">
         <v>410</v>
       </c>
-      <c r="F16" s="45">
+      <c r="F16" s="42">
         <v>400</v>
       </c>
-      <c r="G16" s="45">
+      <c r="G16" s="42">
         <v>390</v>
       </c>
     </row>
     <row r="17" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="39"/>
-      <c r="C17" s="39" t="s">
+      <c r="B17" s="36"/>
+      <c r="C17" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="33">
+      <c r="D17">
         <v>300</v>
       </c>
-      <c r="E17" s="45">
+      <c r="E17" s="42">
         <v>310</v>
       </c>
-      <c r="F17" s="45">
+      <c r="F17" s="42">
         <v>300</v>
       </c>
-      <c r="G17" s="45">
+      <c r="G17" s="42">
         <v>290</v>
       </c>
     </row>
     <row r="18" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="39"/>
-      <c r="C18" s="39" t="s">
+      <c r="B18" s="36"/>
+      <c r="C18" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="33">
+      <c r="D18">
         <v>5000</v>
       </c>
-      <c r="E18" s="45">
+      <c r="E18" s="42">
         <v>5100</v>
       </c>
-      <c r="F18" s="45">
+      <c r="F18" s="42">
         <v>5000</v>
       </c>
-      <c r="G18" s="45">
+      <c r="G18" s="42">
         <v>4900</v>
       </c>
     </row>
     <row r="19" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="39"/>
-      <c r="C19" s="39" t="s">
+      <c r="B19" s="36"/>
+      <c r="C19" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="33">
+      <c r="D19">
         <v>4000</v>
       </c>
-      <c r="E19" s="45">
+      <c r="E19" s="42">
         <v>4100</v>
       </c>
-      <c r="F19" s="45">
+      <c r="F19" s="42">
         <v>4000</v>
       </c>
-      <c r="G19" s="45">
+      <c r="G19" s="42">
         <v>3900</v>
       </c>
     </row>
     <row r="20" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="39"/>
-      <c r="C20" s="39" t="s">
+      <c r="B20" s="36"/>
+      <c r="C20" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="33">
+      <c r="D20">
         <v>2000</v>
       </c>
-      <c r="E20" s="45">
+      <c r="E20" s="42">
         <v>2100</v>
       </c>
-      <c r="F20" s="45">
+      <c r="F20" s="42">
         <v>2000</v>
       </c>
-      <c r="G20" s="45">
+      <c r="G20" s="42">
         <v>1900</v>
       </c>
     </row>
     <row r="21" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="39"/>
-      <c r="C21" s="39" t="s">
+      <c r="B21" s="36"/>
+      <c r="C21" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="33">
+      <c r="D21">
         <v>2000</v>
       </c>
-      <c r="E21" s="45">
+      <c r="E21" s="42">
         <v>2100</v>
       </c>
-      <c r="F21" s="45">
+      <c r="F21" s="42">
         <v>2000</v>
       </c>
-      <c r="G21" s="45">
+      <c r="G21" s="42">
         <v>1900</v>
       </c>
     </row>
     <row r="22" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="39"/>
-      <c r="C22" s="39" t="s">
+      <c r="B22" s="36"/>
+      <c r="C22" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="33">
+      <c r="D22">
         <v>3000</v>
       </c>
-      <c r="E22" s="45">
+      <c r="E22" s="42">
         <v>3100</v>
       </c>
-      <c r="F22" s="45">
+      <c r="F22" s="42">
         <v>3000</v>
       </c>
-      <c r="G22" s="45">
+      <c r="G22" s="42">
         <v>2900</v>
       </c>
     </row>
     <row r="23" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="39"/>
-      <c r="C23" s="39" t="s">
+      <c r="B23" s="36"/>
+      <c r="C23" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="33">
+      <c r="D23">
         <v>4000</v>
       </c>
-      <c r="E23" s="45">
+      <c r="E23" s="42">
         <v>4100</v>
       </c>
-      <c r="F23" s="45">
+      <c r="F23" s="42">
         <v>4000</v>
       </c>
-      <c r="G23" s="45">
+      <c r="G23" s="42">
         <v>3900</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="40" t="s">
+      <c r="B24" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
     </row>
     <row r="25" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="39"/>
-      <c r="C25" s="39" t="s">
+      <c r="B25" s="36"/>
+      <c r="C25" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="D25" s="34">
+      <c r="D25" s="31">
         <v>1828000</v>
       </c>
-      <c r="E25" s="34">
+      <c r="E25" s="31">
         <v>1936970</v>
       </c>
-      <c r="F25" s="34">
+      <c r="F25" s="31">
         <v>1828000</v>
       </c>
-      <c r="G25" s="34">
+      <c r="G25" s="31">
         <v>1731060</v>
       </c>
     </row>
     <row r="26" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="39"/>
-      <c r="C26" s="39" t="s">
+      <c r="B26" s="36"/>
+      <c r="C26" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="34">
+      <c r="D26" s="31">
         <v>480000</v>
       </c>
-      <c r="E26" s="34">
+      <c r="E26" s="31">
         <v>514920</v>
       </c>
-      <c r="F26" s="34">
+      <c r="F26" s="31">
         <v>480000</v>
       </c>
-      <c r="G26" s="34">
+      <c r="G26" s="31">
         <v>451020</v>
       </c>
     </row>
     <row r="27" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="39"/>
-      <c r="C27" s="39" t="s">
+      <c r="B27" s="36"/>
+      <c r="C27" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="34">
+      <c r="D27" s="31">
         <v>644000</v>
       </c>
-      <c r="E27" s="34">
+      <c r="E27" s="31">
         <v>681920</v>
       </c>
-      <c r="F27" s="34">
+      <c r="F27" s="31">
         <v>644000</v>
       </c>
-      <c r="G27" s="34">
+      <c r="G27" s="31">
         <v>611020</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="41"/>
-      <c r="C28" s="41" t="s">
+      <c r="B28" s="38"/>
+      <c r="C28" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="35">
+      <c r="D28" s="32">
         <v>704000</v>
       </c>
-      <c r="E28" s="35">
+      <c r="E28" s="32">
         <v>740130</v>
       </c>
-      <c r="F28" s="35">
+      <c r="F28" s="32">
         <v>704000</v>
       </c>
-      <c r="G28" s="35">
+      <c r="G28" s="32">
         <v>669020</v>
       </c>
     </row>
@@ -2075,75 +2131,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="48"/>
+      <c r="B2" s="45"/>
       <c r="C2" s="1">
         <v>4</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="48"/>
+      <c r="E2" s="45"/>
       <c r="F2" s="2">
         <v>950</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="48"/>
+      <c r="B3" s="45"/>
       <c r="C3" s="1">
         <v>4</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="48"/>
+      <c r="E3" s="45"/>
       <c r="F3" s="2">
         <v>420</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="48"/>
+      <c r="B4" s="45"/>
       <c r="C4" s="1">
         <v>4</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="E4" s="48"/>
+      <c r="E4" s="45"/>
       <c r="F4" s="2">
         <v>899</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="48"/>
+      <c r="B5" s="45"/>
       <c r="C5" s="1">
         <v>4</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D5" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="48"/>
+      <c r="E5" s="45"/>
       <c r="F5" s="2">
         <v>2000</v>
       </c>
@@ -2152,10 +2208,10 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="48"/>
+      <c r="E6" s="45"/>
       <c r="F6" s="2">
         <v>460</v>
       </c>
@@ -2164,21 +2220,21 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="48"/>
+      <c r="E7" s="45"/>
       <c r="F7" s="2">
         <f>C2*F2+C3*F3+C4*F4+C5*F5+F6</f>
         <v>17536</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="B9" s="49"/>
-      <c r="C9" s="49"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
       <c r="D9" s="28" t="s">
         <v>74</v>
       </c>
@@ -2190,11 +2246,11 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
       <c r="D10" s="2">
         <v>950</v>
       </c>
@@ -2206,11 +2262,11 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="45"/>
       <c r="D11" s="2">
         <v>420</v>
       </c>
@@ -2222,11 +2278,11 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="48" t="s">
+      <c r="A12" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="48"/>
-      <c r="C12" s="48"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="45"/>
       <c r="D12" s="2">
         <v>899</v>
       </c>
@@ -2238,11 +2294,11 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="48"/>
-      <c r="C13" s="48"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
       <c r="D13" s="2">
         <v>2000</v>
       </c>
@@ -2254,11 +2310,11 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="48" t="s">
+      <c r="A14" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="B14" s="48"/>
-      <c r="C14" s="48"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="45"/>
       <c r="D14" s="2">
         <v>460</v>
       </c>
@@ -2294,6 +2350,16 @@
     </scenario>
   </scenarios>
   <mergeCells count="17">
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="A9:C9"/>
@@ -2301,16 +2367,6 @@
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2318,65 +2374,235 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D3FF4A0-4423-4038-989D-8989C0888739}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" customWidth="1"/>
+    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="47"/>
+      <c r="B1" s="44"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="47"/>
+      <c r="A2" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="48"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="1">
+        <v>5200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="49" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="1">
+        <v>28.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="49" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="1">
+        <f>B5*B3</f>
+        <v>149760</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="49" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="1">
+        <f>(B5-B4)*B3</f>
+        <v>24960.000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="49" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="1">
+        <f>B4*B3</f>
+        <v>124800</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="49"/>
+      <c r="B9" s="1"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
-      <c r="B10" s="47"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="51"/>
-      <c r="B17" s="51"/>
+      <c r="A10" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="48"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="1">
+        <f>B3</f>
+        <v>5200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="1">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="49" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="1">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="1">
+        <f>B11*B12+B11*B13</f>
+        <v>64480</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="49"/>
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="48"/>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="1">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="1">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="1">
+        <f>SUM(B17:B20)</f>
+        <v>41000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="49"/>
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="48"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" s="1">
+        <f>B8</f>
+        <v>124800</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="1">
+        <f>B21+B14</f>
+        <v>105480</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" s="1">
+        <f>B24-B25</f>
+        <v>19320</v>
+      </c>
+      <c r="C26" s="50">
+        <f>B26/B24</f>
+        <v>0.15480769230769231</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <scenarios current="0" show="0">
+    <scenario name="Поне 15% печалба" locked="1" count="1" user="Lenovo" comment="Created by Lenovo on 09/11/2023_x000a_Modified by Lenovo on 09/11/2023">
+      <inputCells r="B3" val="5200"/>
+    </scenario>
+  </scenarios>
+  <mergeCells count="5">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A23:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="57feac07-fec0-4a43-af96-f48dfa97c0ed" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Документ" ma:contentTypeID="0x0101008D09EBA793C1E143B5F15C3EFFBF29B1" ma:contentTypeVersion="16" ma:contentTypeDescription="Създаване на нов документ" ma:contentTypeScope="" ma:versionID="725d66f9d1cd51d56bd0e502998c711a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="57feac07-fec0-4a43-af96-f48dfa97c0ed" xmlns:ns4="df5d9795-8a9f-4dfc-872e-85e087bd2f0a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="104cc97f392c792fbb3cdbe2738c9ba7" ns3:_="" ns4:_="">
     <xsd:import namespace="57feac07-fec0-4a43-af96-f48dfa97c0ed"/>
@@ -2617,32 +2843,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C452ED50-83D1-4305-B196-CDF3A0F44480}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="df5d9795-8a9f-4dfc-872e-85e087bd2f0a"/>
-    <ds:schemaRef ds:uri="57feac07-fec0-4a43-af96-f48dfa97c0ed"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C6304B0-302C-45F3-86A6-C5084A2DA89E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="57feac07-fec0-4a43-af96-f48dfa97c0ed" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1C1D924-089B-44C0-914D-1598DF899C43}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2659,4 +2877,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C6304B0-302C-45F3-86A6-C5084A2DA89E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C452ED50-83D1-4305-B196-CDF3A0F44480}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="df5d9795-8a9f-4dfc-872e-85e087bd2f0a"/>
+    <ds:schemaRef ds:uri="57feac07-fec0-4a43-af96-f48dfa97c0ed"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>